<commit_message>
Added all smells data
</commit_message>
<xml_diff>
--- a/newData/ALLSmells.xlsx
+++ b/newData/ALLSmells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PP\mvn-project-template\newData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E95B5D4-596F-461C-9BC9-F9CB6C75F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E68834-3360-4E57-9D3D-17D4E04EFF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="228" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -350,7 +350,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -406,7 +406,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>